<commit_message>
ET: SCH/STH fic=x regex issues
</commit_message>
<xml_diff>
--- a/SCH-STH/Baseline Mapping/Ethiopia/eth_sch_sth_remaping_2_registration_202105.xlsx
+++ b/SCH-STH/Baseline Mapping/Ethiopia/eth_sch_sth_remaping_2_registration_202105.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\dsa-forms\SCH-STH\Baseline Mapping\Ethiopia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE4F7D1-FF41-4B02-BEFC-7176DA89E4BE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9654D5CB-76CA-433A-96F4-6036E699F897}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="95">
   <si>
     <t>2. Region</t>
   </si>
@@ -304,9 +304,6 @@
   </si>
   <si>
     <t>Less than 15 years</t>
-  </si>
-  <si>
-    <t>Label with individual ID (Is it possible to generate sample ID values based on individual IDs?)</t>
   </si>
   <si>
     <t>eth_sch_sth_remaping_2_registration_202105</t>
@@ -1030,11 +1027,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomRight" activeCell="D21" sqref="D21:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1251,7 +1248,7 @@
         <v>62</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>4</v>
@@ -1268,7 +1265,7 @@
         <v>62</v>
       </c>
       <c r="B12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>88</v>
@@ -1430,9 +1427,6 @@
       <c r="C21" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="12" t="s">
-        <v>92</v>
-      </c>
       <c r="J21" s="1" t="s">
         <v>72</v>
       </c>
@@ -1446,9 +1440,6 @@
       </c>
       <c r="C22" s="13" t="s">
         <v>21</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>92</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>72</v>
@@ -1621,7 +1612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D1" sqref="D1:E1048576"/>
     </sheetView>
@@ -1740,7 +1731,7 @@
         <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C2">
         <v>202105</v>
@@ -1755,23 +1746,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Flow_SignoffStatus xmlns="4c7bd1d5-db07-43d4-85bd-97d5418eebc6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B9F1557405F204EB54E5AA6C10F8240" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="61e48df3bcdbeb416b226b9b6814dc2c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4c7bd1d5-db07-43d4-85bd-97d5418eebc6" xmlns:ns3="1c1dd18d-f55f-49c2-86f0-6528711f8c6f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ba3abe0560f56dcbf46679ef0c9a9535" ns2:_="" ns3:_="">
     <xsd:import namespace="4c7bd1d5-db07-43d4-85bd-97d5418eebc6"/>
@@ -1994,10 +1968,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Flow_SignoffStatus xmlns="4c7bd1d5-db07-43d4-85bd-97d5418eebc6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{346E3B8A-3A25-4B20-8DFD-2CAF64F2B896}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5F18790-DEA1-4656-A2CA-03E2CC020960}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="4c7bd1d5-db07-43d4-85bd-97d5418eebc6"/>
+    <ds:schemaRef ds:uri="1c1dd18d-f55f-49c2-86f0-6528711f8c6f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2020,20 +2022,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5F18790-DEA1-4656-A2CA-03E2CC020960}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{346E3B8A-3A25-4B20-8DFD-2CAF64F2B896}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="4c7bd1d5-db07-43d4-85bd-97d5418eebc6"/>
-    <ds:schemaRef ds:uri="1c1dd18d-f55f-49c2-86f0-6528711f8c6f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>